<commit_message>
Manejo de operadores entre comillas proveniente de una cadena
</commit_message>
<xml_diff>
--- a/expression_tree_data.xlsx
+++ b/expression_tree_data.xlsx
@@ -759,10 +759,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="107.72265625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="106.5625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="9.9140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="14.078125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="101.48828125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="100.4453125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="10.1875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
se arreglo un cambion de function
</commit_message>
<xml_diff>
--- a/expression_tree_data.xlsx
+++ b/expression_tree_data.xlsx
@@ -759,10 +759,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="14.078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="101.48828125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="100.4453125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="10.1875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="107.72265625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="106.5625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.9140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Imagenes manual de usuario
</commit_message>
<xml_diff>
--- a/expression_tree_data.xlsx
+++ b/expression_tree_data.xlsx
@@ -771,10 +771,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="114.6796875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="106.5625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="9.9140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="14.078125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="108.04296875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="100.4453125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="10.1875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>